<commit_message>
Restored working slate for triggerLogoFlip
</commit_message>
<xml_diff>
--- a/backend/resources/excel/Prizes.xlsx
+++ b/backend/resources/excel/Prizes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17880" windowHeight="12180"/>
+    <workbookView windowWidth="14400" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1257,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1271,7 +1271,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>